<commit_message>
Se contenua con el desarrollo del reporte de orden de produccion. Se programa la parte colaminado.
</commit_message>
<xml_diff>
--- a/Tier.Services/PlantillasReportes/Orden_Produccion.xlsx
+++ b/Tier.Services/PlantillasReportes/Orden_Produccion.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t>Largo</t>
   </si>
@@ -164,9 +164,6 @@
     <t>ACABADO RETIRO:</t>
   </si>
   <si>
-    <t>COLAMINADO</t>
-  </si>
-  <si>
     <t>TROQUELADO</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>Cabida Ancho</t>
+  </si>
+  <si>
+    <t>Paquetes:</t>
   </si>
 </sst>
 </file>
@@ -307,12 +307,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="27">
@@ -605,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -681,6 +687,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -688,6 +697,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -704,11 +716,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,16 +768,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>111311</xdr:colOff>
+      <xdr:colOff>44636</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>142528</xdr:rowOff>
+      <xdr:rowOff>113953</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -791,7 +800,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="142875" y="133350"/>
+          <a:off x="76200" y="142875"/>
           <a:ext cx="682811" cy="390178"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1101,13 +1110,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH41"/>
+  <dimension ref="A1:AH40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="33" width="3" customWidth="1"/>
@@ -1115,7 +1124,7 @@
     <col min="35" max="16384" width="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1154,7 +1163,7 @@
       <c r="AF1" s="33"/>
       <c r="AG1" s="3"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -1193,7 +1202,7 @@
       <c r="AF2" s="36"/>
       <c r="AG2" s="5"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -1230,79 +1239,79 @@
       <c r="AF3" s="40"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
       <c r="AG4" s="9"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
-      <c r="Y5" s="44"/>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="44"/>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="44"/>
-      <c r="AF5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="45"/>
+      <c r="X5" s="45"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="45"/>
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="45"/>
       <c r="AG5" s="11"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="41" t="s">
         <v>8</v>
@@ -1310,19 +1319,19 @@
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
       <c r="E6" s="41"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
       <c r="S6" s="1"/>
       <c r="T6" s="41" t="s">
         <v>9</v>
@@ -1343,7 +1352,7 @@
       <c r="AF6" s="30"/>
       <c r="AG6" s="5"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="41" t="s">
         <v>11</v>
@@ -1351,37 +1360,37 @@
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
       <c r="E7" s="41"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="51"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
       <c r="S7" s="1"/>
       <c r="T7" s="41" t="s">
         <v>12</v>
       </c>
       <c r="U7" s="41"/>
       <c r="V7" s="41"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="42"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="43"/>
+      <c r="Y7" s="43"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="41" t="s">
         <v>13</v>
       </c>
       <c r="AB7" s="41"/>
       <c r="AC7" s="41"/>
-      <c r="AD7" s="42"/>
-      <c r="AE7" s="42"/>
-      <c r="AF7" s="42"/>
+      <c r="AD7" s="43"/>
+      <c r="AE7" s="43"/>
+      <c r="AF7" s="43"/>
       <c r="AG7" s="5"/>
     </row>
     <row r="8" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1419,62 +1428,62 @@
       <c r="AF8" s="28"/>
       <c r="AG8" s="5"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
       <c r="G9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q9" s="47" t="s">
+      <c r="Q9" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47" t="s">
+      <c r="R9" s="49"/>
+      <c r="S9" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47" t="s">
+      <c r="T9" s="49"/>
+      <c r="U9" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z9" s="47" t="s">
+      <c r="Z9" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="AA9" s="47"/>
-      <c r="AB9" s="47" t="s">
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="AC9" s="47"/>
-      <c r="AD9" s="47" t="s">
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="AE9" s="47"/>
-      <c r="AF9" s="47"/>
+      <c r="AE9" s="49"/>
+      <c r="AF9" s="49"/>
       <c r="AG9" s="5"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="41" t="s">
         <v>21</v>
@@ -1515,7 +1524,7 @@
       <c r="AF10" s="36"/>
       <c r="AG10" s="5"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="41" t="s">
         <v>24</v>
@@ -1523,14 +1532,14 @@
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
       <c r="E11" s="41"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
       <c r="N11" s="1"/>
       <c r="O11" s="41" t="s">
         <v>25</v>
@@ -1562,7 +1571,7 @@
       <c r="AF11" s="14"/>
       <c r="AG11" s="5"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="41" t="s">
         <v>28</v>
@@ -1570,14 +1579,14 @@
       <c r="C12" s="41"/>
       <c r="D12" s="41"/>
       <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
       <c r="N12" s="1"/>
       <c r="O12" s="41" t="s">
         <v>29</v>
@@ -1603,7 +1612,7 @@
       <c r="AF12" s="16"/>
       <c r="AG12" s="5"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="41" t="s">
         <v>31</v>
@@ -1611,14 +1620,14 @@
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
       <c r="N13" s="1"/>
       <c r="O13" s="41" t="s">
         <v>32</v>
@@ -1652,31 +1661,31 @@
       <c r="AF13" s="16"/>
       <c r="AG13" s="5"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
       <c r="G14" s="28" t="s">
         <v>36</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="52"/>
       <c r="U14" s="1"/>
       <c r="V14" s="17"/>
       <c r="W14" s="18"/>
@@ -1726,48 +1735,48 @@
       <c r="AF15" s="30"/>
       <c r="AG15" s="7"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="48" t="s">
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
       <c r="S16" s="13"/>
-      <c r="T16" s="48" t="s">
+      <c r="T16" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="U16" s="48"/>
-      <c r="V16" s="48"/>
-      <c r="W16" s="48"/>
-      <c r="X16" s="42"/>
-      <c r="Y16" s="42"/>
-      <c r="Z16" s="42"/>
-      <c r="AA16" s="42"/>
-      <c r="AB16" s="42"/>
-      <c r="AC16" s="42"/>
-      <c r="AD16" s="42"/>
-      <c r="AE16" s="42"/>
-      <c r="AF16" s="42"/>
+      <c r="U16" s="50"/>
+      <c r="V16" s="50"/>
+      <c r="W16" s="50"/>
+      <c r="X16" s="43"/>
+      <c r="Y16" s="43"/>
+      <c r="Z16" s="43"/>
+      <c r="AA16" s="43"/>
+      <c r="AB16" s="43"/>
+      <c r="AC16" s="43"/>
+      <c r="AD16" s="43"/>
+      <c r="AE16" s="43"/>
+      <c r="AF16" s="43"/>
       <c r="AG16" s="20"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="41" t="s">
         <v>40</v>
@@ -1804,7 +1813,7 @@
       <c r="AF17" s="30"/>
       <c r="AG17" s="5"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="21" t="s">
         <v>41</v>
@@ -1813,24 +1822,24 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="48" t="s">
+      <c r="P18" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
-      <c r="U18" s="42"/>
-      <c r="V18" s="42"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
+      <c r="U18" s="43"/>
+      <c r="V18" s="43"/>
       <c r="W18" s="1"/>
       <c r="X18" s="41" t="s">
         <v>43</v>
@@ -1838,14 +1847,14 @@
       <c r="Y18" s="41"/>
       <c r="Z18" s="41"/>
       <c r="AA18" s="41"/>
-      <c r="AB18" s="42"/>
-      <c r="AC18" s="42"/>
-      <c r="AD18" s="42"/>
-      <c r="AE18" s="42"/>
-      <c r="AF18" s="42"/>
+      <c r="AB18" s="43"/>
+      <c r="AC18" s="43"/>
+      <c r="AD18" s="43"/>
+      <c r="AE18" s="43"/>
+      <c r="AF18" s="43"/>
       <c r="AG18" s="5"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="21" t="s">
         <v>44</v>
@@ -1854,24 +1863,24 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
       <c r="O19" s="1"/>
       <c r="P19" s="41" t="s">
         <v>42</v>
       </c>
       <c r="Q19" s="41"/>
       <c r="R19" s="41"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
-      <c r="U19" s="42"/>
-      <c r="V19" s="42"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+      <c r="U19" s="43"/>
+      <c r="V19" s="43"/>
       <c r="W19" s="1"/>
       <c r="X19" s="41" t="s">
         <v>43</v>
@@ -1879,184 +1888,182 @@
       <c r="Y19" s="41"/>
       <c r="Z19" s="41"/>
       <c r="AA19" s="41"/>
-      <c r="AB19" s="42"/>
-      <c r="AC19" s="42"/>
-      <c r="AD19" s="42"/>
-      <c r="AE19" s="42"/>
-      <c r="AF19" s="42"/>
+      <c r="AB19" s="43"/>
+      <c r="AC19" s="43"/>
+      <c r="AD19" s="43"/>
+      <c r="AE19" s="43"/>
+      <c r="AF19" s="43"/>
       <c r="AG19" s="5"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="41" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="G20" s="41"/>
       <c r="H20" s="41"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="30"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
+      <c r="U20" s="43"/>
+      <c r="V20" s="43"/>
       <c r="W20" s="1"/>
       <c r="X20" s="41" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="Y20" s="41"/>
       <c r="Z20" s="41"/>
       <c r="AA20" s="41"/>
-      <c r="AB20" s="42"/>
-      <c r="AC20" s="42"/>
-      <c r="AD20" s="42"/>
-      <c r="AE20" s="42"/>
-      <c r="AF20" s="42"/>
+      <c r="AB20" s="43"/>
+      <c r="AC20" s="43"/>
+      <c r="AD20" s="43"/>
+      <c r="AE20" s="43"/>
+      <c r="AF20" s="43"/>
       <c r="AG20" s="5"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="41" t="s">
+    <row r="21" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="40"/>
+      <c r="X21" s="40"/>
+      <c r="Y21" s="40"/>
+      <c r="Z21" s="40"/>
+      <c r="AA21" s="40"/>
+      <c r="AB21" s="40"/>
+      <c r="AC21" s="40"/>
+      <c r="AD21" s="40"/>
+      <c r="AE21" s="40"/>
+      <c r="AF21" s="40"/>
+      <c r="AG21" s="7"/>
+    </row>
+    <row r="22" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
-      <c r="S21" s="42"/>
-      <c r="T21" s="42"/>
-      <c r="U21" s="42"/>
-      <c r="V21" s="42"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="41" t="s">
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="Y21" s="41"/>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="41"/>
-      <c r="AB21" s="42"/>
-      <c r="AC21" s="42"/>
-      <c r="AD21" s="42"/>
-      <c r="AE21" s="42"/>
-      <c r="AF21" s="42"/>
-      <c r="AG21" s="5"/>
-    </row>
-    <row r="22" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
-      <c r="S22" s="40"/>
-      <c r="T22" s="40"/>
-      <c r="U22" s="40"/>
-      <c r="V22" s="40"/>
-      <c r="W22" s="40"/>
-      <c r="X22" s="40"/>
-      <c r="Y22" s="40"/>
-      <c r="Z22" s="40"/>
-      <c r="AA22" s="40"/>
-      <c r="AB22" s="40"/>
-      <c r="AC22" s="40"/>
-      <c r="AD22" s="40"/>
-      <c r="AE22" s="40"/>
-      <c r="AF22" s="40"/>
-      <c r="AG22" s="7"/>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="48" t="s">
+      <c r="Y22" s="50"/>
+      <c r="Z22" s="50"/>
+      <c r="AA22" s="50"/>
+      <c r="AB22" s="43"/>
+      <c r="AC22" s="43"/>
+      <c r="AD22" s="43"/>
+      <c r="AE22" s="43"/>
+      <c r="AF22" s="43"/>
+      <c r="AG22" s="20"/>
+    </row>
+    <row r="23" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="42"/>
-      <c r="U23" s="42"/>
-      <c r="V23" s="42"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y23" s="48"/>
-      <c r="Z23" s="48"/>
-      <c r="AA23" s="48"/>
-      <c r="AB23" s="42"/>
-      <c r="AC23" s="42"/>
-      <c r="AD23" s="42"/>
-      <c r="AE23" s="42"/>
-      <c r="AF23" s="42"/>
-      <c r="AG23" s="20"/>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="S23" s="47"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="47"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
+      <c r="Z23" s="30"/>
+      <c r="AA23" s="30"/>
+      <c r="AB23" s="30"/>
+      <c r="AC23" s="30"/>
+      <c r="AD23" s="30"/>
+      <c r="AE23" s="30"/>
+      <c r="AF23" s="30"/>
+      <c r="AG23" s="5"/>
+    </row>
+    <row r="24" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="30" t="s">
-        <v>30</v>
-      </c>
+      <c r="B24" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="30"/>
       <c r="H24" s="30"/>
       <c r="I24" s="30"/>
@@ -2067,13 +2074,11 @@
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
       <c r="P24" s="30"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="S24" s="45"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="45"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
       <c r="V24" s="30"/>
       <c r="W24" s="30"/>
       <c r="X24" s="30"/>
@@ -2087,105 +2092,111 @@
       <c r="AF24" s="30"/>
       <c r="AG24" s="5"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="30"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="30"/>
-      <c r="AB25" s="30"/>
-      <c r="AC25" s="30"/>
-      <c r="AD25" s="30"/>
-      <c r="AE25" s="30"/>
-      <c r="AF25" s="30"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="43"/>
+      <c r="U25" s="43"/>
+      <c r="V25" s="43"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y25" s="50"/>
+      <c r="Z25" s="50"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="43"/>
+      <c r="AC25" s="43"/>
+      <c r="AD25" s="43"/>
+      <c r="AE25" s="43"/>
+      <c r="AF25" s="1"/>
       <c r="AG25" s="5"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
+      <c r="B26" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="41" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
       <c r="I26" s="41"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
       <c r="N26" s="1"/>
       <c r="O26" s="41" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="P26" s="41"/>
       <c r="Q26" s="41"/>
       <c r="R26" s="41"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
-      <c r="U26" s="42"/>
-      <c r="V26" s="42"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
       <c r="W26" s="1"/>
-      <c r="X26" s="28"/>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="28"/>
-      <c r="AA26" s="28"/>
-      <c r="AB26" s="28"/>
-      <c r="AC26" s="28"/>
-      <c r="AD26" s="28"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
+      <c r="X26" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y26" s="41"/>
+      <c r="Z26" s="41"/>
+      <c r="AA26" s="41"/>
+      <c r="AB26" s="30"/>
+      <c r="AC26" s="30"/>
+      <c r="AD26" s="30"/>
+      <c r="AE26" s="30"/>
+      <c r="AF26" s="1"/>
       <c r="AG26" s="5"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
       <c r="F27" s="41" t="s">
         <v>58</v>
       </c>
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
       <c r="I27" s="41"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
       <c r="N27" s="1"/>
       <c r="O27" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P27" s="41"/>
       <c r="Q27" s="41"/>
@@ -2196,132 +2207,126 @@
       <c r="V27" s="30"/>
       <c r="W27" s="1"/>
       <c r="X27" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y27" s="41"/>
       <c r="Z27" s="41"/>
       <c r="AA27" s="41"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="30"/>
-      <c r="AE27" s="30"/>
+      <c r="AB27" s="43"/>
+      <c r="AC27" s="43"/>
+      <c r="AD27" s="43"/>
+      <c r="AE27" s="43"/>
       <c r="AF27" s="1"/>
       <c r="AG27" s="5"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
+    <row r="28" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
       <c r="S28" s="30"/>
       <c r="T28" s="30"/>
       <c r="U28" s="30"/>
       <c r="V28" s="30"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="41" t="s">
+      <c r="W28" s="30"/>
+      <c r="X28" s="30"/>
+      <c r="Y28" s="30"/>
+      <c r="Z28" s="30"/>
+      <c r="AA28" s="30"/>
+      <c r="AB28" s="30"/>
+      <c r="AC28" s="30"/>
+      <c r="AD28" s="30"/>
+      <c r="AE28" s="30"/>
+      <c r="AF28" s="30"/>
+      <c r="AG28" s="7"/>
+    </row>
+    <row r="29" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Y28" s="41"/>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="41"/>
-      <c r="AB28" s="42"/>
-      <c r="AC28" s="42"/>
-      <c r="AD28" s="42"/>
-      <c r="AE28" s="42"/>
-      <c r="AF28" s="1"/>
-      <c r="AG28" s="5"/>
-    </row>
-    <row r="29" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="30"/>
-      <c r="V29" s="30"/>
-      <c r="W29" s="30"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="30"/>
-      <c r="Z29" s="30"/>
-      <c r="AA29" s="30"/>
-      <c r="AB29" s="30"/>
-      <c r="AC29" s="30"/>
-      <c r="AD29" s="30"/>
-      <c r="AE29" s="30"/>
-      <c r="AF29" s="30"/>
-      <c r="AG29" s="7"/>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="48"/>
-      <c r="S30" s="48"/>
-      <c r="T30" s="48"/>
-      <c r="U30" s="48"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="48"/>
-      <c r="AA30" s="48"/>
-      <c r="AB30" s="48"/>
-      <c r="AC30" s="48"/>
-      <c r="AD30" s="48"/>
-      <c r="AE30" s="48"/>
-      <c r="AF30" s="48"/>
-      <c r="AG30" s="20"/>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="50"/>
+      <c r="AA29" s="50"/>
+      <c r="AB29" s="50"/>
+      <c r="AC29" s="50"/>
+      <c r="AD29" s="50"/>
+      <c r="AE29" s="50"/>
+      <c r="AF29" s="50"/>
+      <c r="AG29" s="20"/>
+    </row>
+    <row r="30" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="41"/>
+      <c r="U30" s="41"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="41"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="41"/>
+      <c r="Z30" s="41"/>
+      <c r="AA30" s="41"/>
+      <c r="AB30" s="41"/>
+      <c r="AC30" s="41"/>
+      <c r="AD30" s="41"/>
+      <c r="AE30" s="41"/>
+      <c r="AF30" s="41"/>
+      <c r="AG30" s="5"/>
+    </row>
+    <row r="31" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="41"/>
       <c r="C31" s="41"/>
@@ -2356,7 +2361,7 @@
       <c r="AF31" s="41"/>
       <c r="AG31" s="5"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="41"/>
       <c r="C32" s="41"/>
@@ -2391,132 +2396,144 @@
       <c r="AF32" s="41"/>
       <c r="AG32" s="5"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41"/>
-      <c r="Q33" s="41"/>
-      <c r="R33" s="41"/>
-      <c r="S33" s="41"/>
-      <c r="T33" s="41"/>
-      <c r="U33" s="41"/>
-      <c r="V33" s="41"/>
-      <c r="W33" s="41"/>
-      <c r="X33" s="41"/>
-      <c r="Y33" s="41"/>
-      <c r="Z33" s="41"/>
-      <c r="AA33" s="41"/>
-      <c r="AB33" s="41"/>
-      <c r="AC33" s="41"/>
-      <c r="AD33" s="41"/>
-      <c r="AE33" s="41"/>
-      <c r="AF33" s="41"/>
-      <c r="AG33" s="5"/>
-    </row>
-    <row r="34" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="U34" s="18"/>
-      <c r="V34" s="18"/>
-      <c r="W34" s="18"/>
-      <c r="X34" s="18"/>
-      <c r="Y34" s="18"/>
-      <c r="Z34" s="18"/>
-      <c r="AA34" s="18"/>
-      <c r="AB34" s="18"/>
-      <c r="AC34" s="18"/>
-      <c r="AD34" s="18"/>
-      <c r="AE34" s="18"/>
-      <c r="AF34" s="18"/>
-      <c r="AG34" s="7"/>
-    </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="49" t="s">
+    <row r="33" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
+      <c r="V33" s="18"/>
+      <c r="W33" s="18"/>
+      <c r="X33" s="18"/>
+      <c r="Y33" s="18"/>
+      <c r="Z33" s="18"/>
+      <c r="AA33" s="18"/>
+      <c r="AB33" s="18"/>
+      <c r="AC33" s="18"/>
+      <c r="AD33" s="18"/>
+      <c r="AE33" s="18"/>
+      <c r="AF33" s="18"/>
+      <c r="AG33" s="7"/>
+    </row>
+    <row r="34" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="48" t="s">
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="49" t="s">
+      <c r="N34" s="51"/>
+      <c r="O34" s="51"/>
+      <c r="P34" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="N35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="48" t="s">
+      <c r="Q34" s="50"/>
+      <c r="R34" s="50"/>
+      <c r="S34" s="50"/>
+      <c r="T34" s="50"/>
+      <c r="U34" s="50"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="Q35" s="48"/>
-      <c r="R35" s="48"/>
-      <c r="S35" s="48"/>
-      <c r="T35" s="48"/>
-      <c r="U35" s="48"/>
-      <c r="V35" s="13"/>
-      <c r="W35" s="49" t="s">
+      <c r="X34" s="51"/>
+      <c r="Y34" s="51"/>
+      <c r="Z34" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="49"/>
-      <c r="Z35" s="48" t="s">
+      <c r="AA34" s="50"/>
+      <c r="AB34" s="50"/>
+      <c r="AC34" s="50"/>
+      <c r="AD34" s="50"/>
+      <c r="AE34" s="50"/>
+      <c r="AF34" s="50"/>
+      <c r="AG34" s="20"/>
+    </row>
+    <row r="35" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="AA35" s="48"/>
-      <c r="AB35" s="48"/>
-      <c r="AC35" s="48"/>
-      <c r="AD35" s="48"/>
-      <c r="AE35" s="48"/>
-      <c r="AF35" s="48"/>
-      <c r="AG35" s="20"/>
-    </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="41"/>
+      <c r="S35" s="41"/>
+      <c r="T35" s="41"/>
+      <c r="U35" s="41"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="X35" s="47"/>
+      <c r="Y35" s="47"/>
+      <c r="Z35" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA35" s="41"/>
+      <c r="AB35" s="41"/>
+      <c r="AC35" s="41"/>
+      <c r="AD35" s="41"/>
+      <c r="AE35" s="41"/>
+      <c r="AF35" s="41"/>
+      <c r="AG35" s="5"/>
+    </row>
+    <row r="36" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
+      <c r="B36" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="41" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F36" s="41"/>
       <c r="G36" s="41"/>
@@ -2525,13 +2542,13 @@
       <c r="J36" s="41"/>
       <c r="K36" s="41"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
+      <c r="M36" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
       <c r="P36" s="41" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Q36" s="41"/>
       <c r="R36" s="41"/>
@@ -2539,13 +2556,13 @@
       <c r="T36" s="41"/>
       <c r="U36" s="41"/>
       <c r="V36" s="1"/>
-      <c r="W36" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="X36" s="45"/>
-      <c r="Y36" s="45"/>
+      <c r="W36" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="X36" s="47"/>
+      <c r="Y36" s="47"/>
       <c r="Z36" s="41" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="AA36" s="41"/>
       <c r="AB36" s="41"/>
@@ -2555,15 +2572,15 @@
       <c r="AF36" s="41"/>
       <c r="AG36" s="5"/>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
+      <c r="B37" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
       <c r="E37" s="41" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="F37" s="41"/>
       <c r="G37" s="41"/>
@@ -2572,13 +2589,13 @@
       <c r="J37" s="41"/>
       <c r="K37" s="41"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
+      <c r="M37" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="N37" s="47"/>
+      <c r="O37" s="47"/>
       <c r="P37" s="41" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="Q37" s="41"/>
       <c r="R37" s="41"/>
@@ -2586,11 +2603,11 @@
       <c r="T37" s="41"/>
       <c r="U37" s="41"/>
       <c r="V37" s="1"/>
-      <c r="W37" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="45"/>
+      <c r="W37" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="X37" s="47"/>
+      <c r="Y37" s="47"/>
       <c r="Z37" s="41" t="s">
         <v>78</v>
       </c>
@@ -2602,15 +2619,15 @@
       <c r="AF37" s="41"/>
       <c r="AG37" s="5"/>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
+      <c r="B38" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
       <c r="E38" s="41" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="F38" s="41"/>
       <c r="G38" s="41"/>
@@ -2619,121 +2636,68 @@
       <c r="J38" s="41"/>
       <c r="K38" s="41"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="41"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
       <c r="V38" s="1"/>
-      <c r="W38" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="X38" s="45"/>
-      <c r="Y38" s="45"/>
-      <c r="Z38" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA38" s="41"/>
-      <c r="AB38" s="41"/>
-      <c r="AC38" s="41"/>
-      <c r="AD38" s="41"/>
-      <c r="AE38" s="41"/>
-      <c r="AF38" s="41"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
       <c r="AG38" s="5"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
-      <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-      <c r="AF39" s="1"/>
-      <c r="AG39" s="5"/>
-    </row>
-    <row r="40" spans="1:33" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="24"/>
-      <c r="P40" s="24"/>
-      <c r="Q40" s="24"/>
-      <c r="R40" s="24"/>
-      <c r="S40" s="24"/>
-      <c r="T40" s="24"/>
-      <c r="U40" s="24"/>
-      <c r="V40" s="24"/>
-      <c r="W40" s="24"/>
-      <c r="X40" s="24"/>
-      <c r="Y40" s="24"/>
-      <c r="Z40" s="24"/>
-      <c r="AA40" s="24"/>
-      <c r="AB40" s="24"/>
-      <c r="AC40" s="24"/>
-      <c r="AD40" s="24"/>
-      <c r="AE40" s="24"/>
-      <c r="AF40" s="24"/>
-      <c r="AG40" s="25"/>
-    </row>
-    <row r="41" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:33" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="24"/>
+      <c r="Q39" s="24"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="24"/>
+      <c r="T39" s="24"/>
+      <c r="U39" s="24"/>
+      <c r="V39" s="24"/>
+      <c r="W39" s="24"/>
+      <c r="X39" s="24"/>
+      <c r="Y39" s="24"/>
+      <c r="Z39" s="24"/>
+      <c r="AA39" s="24"/>
+      <c r="AB39" s="24"/>
+      <c r="AC39" s="24"/>
+      <c r="AD39" s="24"/>
+      <c r="AE39" s="24"/>
+      <c r="AF39" s="24"/>
+      <c r="AG39" s="25"/>
+    </row>
+    <row r="40" spans="1:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="144">
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:K39"/>
+  <mergeCells count="141">
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="E38:K38"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="P38:U38"/>
-    <mergeCell ref="W38:Y38"/>
-    <mergeCell ref="Z38:AF38"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="E37:K37"/>
     <mergeCell ref="M37:O37"/>
@@ -2752,59 +2716,61 @@
     <mergeCell ref="P35:U35"/>
     <mergeCell ref="W35:Y35"/>
     <mergeCell ref="Z35:AF35"/>
-    <mergeCell ref="AB28:AE28"/>
-    <mergeCell ref="B29:AF29"/>
-    <mergeCell ref="G30:AF30"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:K34"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="P34:U34"/>
+    <mergeCell ref="W34:Y34"/>
+    <mergeCell ref="Z34:AF34"/>
+    <mergeCell ref="AB27:AE27"/>
+    <mergeCell ref="B28:AF28"/>
+    <mergeCell ref="G29:AF29"/>
+    <mergeCell ref="B30:AF30"/>
     <mergeCell ref="B31:AF31"/>
     <mergeCell ref="B32:AF32"/>
-    <mergeCell ref="B33:AF33"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="O28:R28"/>
-    <mergeCell ref="S28:V28"/>
-    <mergeCell ref="X28:AA28"/>
-    <mergeCell ref="X26:AF26"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="J27:M27"/>
     <mergeCell ref="O27:R27"/>
     <mergeCell ref="S27:V27"/>
     <mergeCell ref="X27:AA27"/>
-    <mergeCell ref="AB27:AE27"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:P24"/>
-    <mergeCell ref="R24:U24"/>
-    <mergeCell ref="V24:AF24"/>
-    <mergeCell ref="F25:AF25"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="F26:I26"/>
     <mergeCell ref="J26:M26"/>
     <mergeCell ref="O26:R26"/>
     <mergeCell ref="S26:V26"/>
-    <mergeCell ref="AB21:AF21"/>
-    <mergeCell ref="B22:AF22"/>
+    <mergeCell ref="X26:AA26"/>
+    <mergeCell ref="AB26:AE26"/>
     <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:V23"/>
-    <mergeCell ref="X23:AA23"/>
-    <mergeCell ref="AB23:AF23"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="S21:V21"/>
-    <mergeCell ref="X21:AA21"/>
+    <mergeCell ref="F23:P23"/>
+    <mergeCell ref="R23:U23"/>
+    <mergeCell ref="V23:AF23"/>
+    <mergeCell ref="F24:AF24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="O25:R25"/>
+    <mergeCell ref="S25:V25"/>
+    <mergeCell ref="AB25:AE25"/>
+    <mergeCell ref="X25:Z25"/>
     <mergeCell ref="G19:N19"/>
     <mergeCell ref="P19:R19"/>
     <mergeCell ref="S19:V19"/>
     <mergeCell ref="X19:AA19"/>
     <mergeCell ref="AB19:AF19"/>
+    <mergeCell ref="AB20:AF20"/>
+    <mergeCell ref="B21:AF21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:V22"/>
+    <mergeCell ref="X22:AA22"/>
+    <mergeCell ref="AB22:AF22"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:V20"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="S20:V20"/>
     <mergeCell ref="X20:AA20"/>
-    <mergeCell ref="AB20:AF20"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="G18:N18"/>
     <mergeCell ref="P18:R18"/>
@@ -2813,7 +2779,6 @@
     <mergeCell ref="AB18:AF18"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K14:T14"/>
     <mergeCell ref="B15:AF15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="G16:I16"/>
@@ -2822,6 +2787,8 @@
     <mergeCell ref="X16:AF16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:AF17"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="O14:T14"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="F12:M12"/>
     <mergeCell ref="O12:Q12"/>

</xml_diff>